<commit_message>
testng dataprovider examples added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFolder/username_password.xlsx
+++ b/src/test/resources/ExcelFolder/username_password.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enkhb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enkhb\rest_assured\apachePOI_Practice\src\test\resources\ExcelFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8215C2BA-4E91-4D64-B3E0-D87B266B05C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49D0770-F2EF-47B8-8464-6B5FFB5CFE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="4890" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8700" yWindow="3075" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,37 +25,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>pass123</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Integer</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>three</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +60,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,13 +90,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,30 +381,33 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H9" sqref="H9:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -403,7 +418,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>